<commit_message>
[Completo] ajuste da importação
</commit_message>
<xml_diff>
--- a/src/infoinvestbr/src/analise/rendavariavel.xlsx
+++ b/src/infoinvestbr/src/analise/rendavariavel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\Projeto TCC\src\infoinvestbr\src\analise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DCCAEA-0A14-484E-BF53-E76B2518A43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA02586E-E46C-424E-99DF-0EAD882BBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE4D7603-F5DE-4554-98D0-6C8EE02FCDF4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{FE4D7603-F5DE-4554-98D0-6C8EE02FCDF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ações" sheetId="1" r:id="rId1"/>
@@ -7762,29 +7762,31 @@
   <dimension ref="A1:Y437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="Y1" sqref="A1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="8.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="16" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
     <col min="21" max="21" width="27.85546875" customWidth="1"/>
     <col min="22" max="22" width="30.5703125" style="8" customWidth="1"/>
     <col min="23" max="23" width="61.5703125" customWidth="1"/>
@@ -7946,7 +7948,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>241</v>
       </c>
@@ -8177,7 +8179,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>200</v>
       </c>
@@ -8254,7 +8256,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="7" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>191</v>
       </c>
@@ -8780,8 +8782,11 @@
       <c r="X13" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>219</v>
       </c>
@@ -8858,7 +8863,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -8931,8 +8936,11 @@
       <c r="X15" t="s">
         <v>1131</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y15">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -9005,8 +9013,11 @@
       <c r="X16" t="s">
         <v>1131</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -9078,6 +9089,9 @@
       </c>
       <c r="X17" t="s">
         <v>1131</v>
+      </c>
+      <c r="Y17">
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -9154,7 +9168,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -9226,6 +9240,9 @@
       </c>
       <c r="X19" t="s">
         <v>1135</v>
+      </c>
+      <c r="Y19">
+        <v>613</v>
       </c>
     </row>
     <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -9376,7 +9393,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>358</v>
       </c>
@@ -9748,6 +9765,9 @@
       <c r="X26" t="s">
         <v>1149</v>
       </c>
+      <c r="Y26">
+        <v>173</v>
+      </c>
     </row>
     <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -9826,7 +9846,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -9898,6 +9918,9 @@
       </c>
       <c r="X28" t="s">
         <v>1786</v>
+      </c>
+      <c r="Y28">
+        <v>899</v>
       </c>
     </row>
     <row r="29" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -10047,6 +10070,9 @@
       <c r="X30" t="s">
         <v>1153</v>
       </c>
+      <c r="Y30">
+        <v>163</v>
+      </c>
     </row>
     <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -10121,6 +10147,9 @@
       <c r="X31" t="s">
         <v>1153</v>
       </c>
+      <c r="Y31">
+        <v>163</v>
+      </c>
     </row>
     <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -10195,8 +10224,11 @@
       <c r="X32" t="s">
         <v>1155</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>416</v>
       </c>
@@ -10420,6 +10452,9 @@
       <c r="X35" t="s">
         <v>1161</v>
       </c>
+      <c r="Y35">
+        <v>421</v>
+      </c>
     </row>
     <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -10494,6 +10529,9 @@
       <c r="X36" t="s">
         <v>1161</v>
       </c>
+      <c r="Y36">
+        <v>421</v>
+      </c>
     </row>
     <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -10569,7 +10607,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -10646,7 +10684,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>238</v>
       </c>
@@ -10723,7 +10761,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>248</v>
       </c>
@@ -10800,7 +10838,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>255</v>
       </c>
@@ -10877,7 +10915,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>354</v>
       </c>
@@ -11027,6 +11065,9 @@
       <c r="X43" t="s">
         <v>1174</v>
       </c>
+      <c r="Y43">
+        <v>180</v>
+      </c>
     </row>
     <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -11101,6 +11142,9 @@
       <c r="X44" t="s">
         <v>1174</v>
       </c>
+      <c r="Y44">
+        <v>180</v>
+      </c>
     </row>
     <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -11176,7 +11220,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>249</v>
       </c>
@@ -11253,7 +11297,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>256</v>
       </c>
@@ -11330,7 +11374,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>239</v>
       </c>
@@ -11558,7 +11602,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -11635,7 +11679,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>242</v>
       </c>
@@ -11712,7 +11756,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>243</v>
       </c>
@@ -11789,7 +11833,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>269</v>
       </c>
@@ -11862,8 +11906,11 @@
       <c r="X54" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y54">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>252</v>
       </c>
@@ -11935,6 +11982,9 @@
       </c>
       <c r="X55" t="s">
         <v>1191</v>
+      </c>
+      <c r="Y55">
+        <v>337</v>
       </c>
     </row>
     <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -12088,7 +12138,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -12162,7 +12212,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>415</v>
       </c>
@@ -12310,7 +12360,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>270</v>
       </c>
@@ -12387,7 +12437,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>274</v>
       </c>
@@ -12464,7 +12514,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -12541,7 +12591,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>268</v>
       </c>
@@ -12772,7 +12822,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>259</v>
       </c>
@@ -12923,7 +12973,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>348</v>
       </c>
@@ -13000,7 +13050,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>352</v>
       </c>
@@ -13077,7 +13127,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>350</v>
       </c>
@@ -13154,7 +13204,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>353</v>
       </c>
@@ -13231,7 +13281,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>351</v>
       </c>
@@ -13385,7 +13435,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -13462,7 +13512,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>254</v>
       </c>
@@ -13770,7 +13820,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -13847,7 +13897,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>250</v>
       </c>
@@ -13924,7 +13974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>267</v>
       </c>
@@ -14001,7 +14051,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>246</v>
       </c>
@@ -14078,7 +14128,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>275</v>
       </c>
@@ -14155,7 +14205,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>273</v>
       </c>
@@ -14608,7 +14658,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="91" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -14680,6 +14730,9 @@
       </c>
       <c r="X91" t="s">
         <v>1237</v>
+      </c>
+      <c r="Y91">
+        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -14755,6 +14808,9 @@
       <c r="X92" t="s">
         <v>1239</v>
       </c>
+      <c r="Y92">
+        <v>198</v>
+      </c>
     </row>
     <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
@@ -14830,7 +14886,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="94" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>151</v>
       </c>
@@ -14903,8 +14959,11 @@
       <c r="X94" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y94">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -14977,8 +15036,11 @@
       <c r="X95" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y95">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>152</v>
       </c>
@@ -15050,6 +15112,9 @@
       </c>
       <c r="X96" t="s">
         <v>1243</v>
+      </c>
+      <c r="Y96">
+        <v>454</v>
       </c>
     </row>
     <row r="97" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -15200,7 +15265,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="99" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>162</v>
       </c>
@@ -15273,8 +15338,11 @@
       <c r="X99" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y99">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>157</v>
       </c>
@@ -15347,8 +15415,11 @@
       <c r="X100" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y100">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>171</v>
       </c>
@@ -15421,8 +15492,11 @@
       <c r="X101" t="s">
         <v>1249</v>
       </c>
-    </row>
-    <row r="102" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y101">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>223</v>
       </c>
@@ -15495,8 +15569,11 @@
       <c r="X102" t="s">
         <v>1251</v>
       </c>
-    </row>
-    <row r="103" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y102">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>224</v>
       </c>
@@ -15568,6 +15645,9 @@
       </c>
       <c r="X103" t="s">
         <v>1251</v>
+      </c>
+      <c r="Y103">
+        <v>482</v>
       </c>
     </row>
     <row r="104" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -15718,7 +15798,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>414</v>
       </c>
@@ -15795,7 +15875,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>412</v>
       </c>
@@ -15869,7 +15949,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="108" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>148</v>
       </c>
@@ -15942,8 +16022,11 @@
       <c r="X108" t="s">
         <v>1259</v>
       </c>
-    </row>
-    <row r="109" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y108">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>149</v>
       </c>
@@ -16016,8 +16099,11 @@
       <c r="X109" t="s">
         <v>1259</v>
       </c>
-    </row>
-    <row r="110" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y109">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>181</v>
       </c>
@@ -16090,8 +16176,11 @@
       <c r="X110" t="s">
         <v>1261</v>
       </c>
-    </row>
-    <row r="111" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y110">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>160</v>
       </c>
@@ -16163,6 +16252,9 @@
       </c>
       <c r="X111" t="s">
         <v>1261</v>
+      </c>
+      <c r="Y111">
+        <v>455</v>
       </c>
     </row>
     <row r="112" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -16242,7 +16334,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="113" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>165</v>
       </c>
@@ -16315,8 +16407,11 @@
       <c r="X113" t="s">
         <v>1265</v>
       </c>
-    </row>
-    <row r="114" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y113">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>155</v>
       </c>
@@ -16388,6 +16483,9 @@
       </c>
       <c r="X114" t="s">
         <v>1265</v>
+      </c>
+      <c r="Y114">
+        <v>457</v>
       </c>
     </row>
     <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -16464,7 +16562,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="116" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>163</v>
       </c>
@@ -16537,8 +16635,11 @@
       <c r="X116" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="117" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y116">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>196</v>
       </c>
@@ -16611,8 +16712,11 @@
       <c r="X117" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="118" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y117">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>194</v>
       </c>
@@ -16685,8 +16789,11 @@
       <c r="X118" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="119" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y118">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>202</v>
       </c>
@@ -16759,8 +16866,11 @@
       <c r="X119" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="120" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y119">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>197</v>
       </c>
@@ -16832,6 +16942,9 @@
       </c>
       <c r="X120" t="s">
         <v>1271</v>
+      </c>
+      <c r="Y120">
+        <v>462</v>
       </c>
     </row>
     <row r="121" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -16982,7 +17095,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>271</v>
       </c>
@@ -17059,7 +17172,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>272</v>
       </c>
@@ -17290,7 +17403,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>355</v>
       </c>
@@ -17367,7 +17480,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>357</v>
       </c>
@@ -17595,7 +17708,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="131" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>32</v>
       </c>
@@ -17667,6 +17780,9 @@
       </c>
       <c r="X131" t="s">
         <v>1287</v>
+      </c>
+      <c r="Y131">
+        <v>442</v>
       </c>
     </row>
     <row r="132" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -17746,7 +17862,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="133" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>173</v>
       </c>
@@ -17819,8 +17935,11 @@
       <c r="X133" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="134" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y133">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>164</v>
       </c>
@@ -17893,8 +18012,11 @@
       <c r="X134" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="135" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y134">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>166</v>
       </c>
@@ -17966,6 +18088,9 @@
       </c>
       <c r="X135" t="s">
         <v>1291</v>
+      </c>
+      <c r="Y135">
+        <v>459</v>
       </c>
     </row>
     <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -18041,6 +18166,9 @@
       <c r="X136" t="s">
         <v>1788</v>
       </c>
+      <c r="Y136">
+        <v>170</v>
+      </c>
     </row>
     <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -18560,7 +18688,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>349</v>
       </c>
@@ -19093,7 +19221,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>240</v>
       </c>
@@ -19462,6 +19590,9 @@
       <c r="X155" t="s">
         <v>1321</v>
       </c>
+      <c r="Y155">
+        <v>171</v>
+      </c>
     </row>
     <row r="156" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
@@ -19613,6 +19744,9 @@
       <c r="X157" t="s">
         <v>1325</v>
       </c>
+      <c r="Y157">
+        <v>181</v>
+      </c>
     </row>
     <row r="158" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -19687,6 +19821,9 @@
       <c r="X158" t="s">
         <v>1325</v>
       </c>
+      <c r="Y158">
+        <v>181</v>
+      </c>
     </row>
     <row r="159" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
@@ -19761,8 +19898,11 @@
       <c r="X159" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="160" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y159">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>185</v>
       </c>
@@ -19835,8 +19975,11 @@
       <c r="X160" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="161" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y160">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>169</v>
       </c>
@@ -19909,8 +20052,11 @@
       <c r="X161" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="162" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y161">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>170</v>
       </c>
@@ -19983,8 +20129,11 @@
       <c r="X162" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="163" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y162">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>195</v>
       </c>
@@ -20057,8 +20206,11 @@
       <c r="X163" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="164" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y163">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>201</v>
       </c>
@@ -20131,8 +20283,11 @@
       <c r="X164" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="165" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y164">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>198</v>
       </c>
@@ -20204,6 +20359,9 @@
       </c>
       <c r="X165" t="s">
         <v>1333</v>
+      </c>
+      <c r="Y165">
+        <v>448</v>
       </c>
     </row>
     <row r="166" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -20283,7 +20441,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="167" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>192</v>
       </c>
@@ -20355,6 +20513,9 @@
       </c>
       <c r="X167" t="s">
         <v>1337</v>
+      </c>
+      <c r="Y167">
+        <v>469</v>
       </c>
     </row>
     <row r="168" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -20430,6 +20591,9 @@
       <c r="X168" t="s">
         <v>1339</v>
       </c>
+      <c r="Y168">
+        <v>190</v>
+      </c>
     </row>
     <row r="169" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
@@ -20508,7 +20672,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="170" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>187</v>
       </c>
@@ -20581,8 +20745,11 @@
       <c r="X170" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="171" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y170">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>193</v>
       </c>
@@ -20655,8 +20822,11 @@
       <c r="X171" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="172" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y171">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>167</v>
       </c>
@@ -20729,8 +20899,11 @@
       <c r="X172" t="s">
         <v>1347</v>
       </c>
-    </row>
-    <row r="173" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y172">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>184</v>
       </c>
@@ -20803,8 +20976,11 @@
       <c r="X173" t="s">
         <v>1347</v>
       </c>
-    </row>
-    <row r="174" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y173">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>158</v>
       </c>
@@ -20876,6 +21052,9 @@
       </c>
       <c r="X174" t="s">
         <v>1347</v>
+      </c>
+      <c r="Y174">
+        <v>471</v>
       </c>
     </row>
     <row r="175" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -20955,7 +21134,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="176" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>189</v>
       </c>
@@ -21028,8 +21207,11 @@
       <c r="X176" t="s">
         <v>1351</v>
       </c>
-    </row>
-    <row r="177" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y176">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>190</v>
       </c>
@@ -21101,6 +21283,9 @@
       </c>
       <c r="X177" t="s">
         <v>1351</v>
+      </c>
+      <c r="Y177">
+        <v>470</v>
       </c>
     </row>
     <row r="178" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -21177,7 +21362,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="179" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>161</v>
       </c>
@@ -21250,8 +21435,11 @@
       <c r="X179" t="s">
         <v>1355</v>
       </c>
-    </row>
-    <row r="180" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y179">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
@@ -21324,8 +21512,11 @@
       <c r="X180" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="181" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y180">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -21398,8 +21589,11 @@
       <c r="X181" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="182" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y181">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>186</v>
       </c>
@@ -21471,6 +21665,9 @@
       </c>
       <c r="X182" t="s">
         <v>1359</v>
+      </c>
+      <c r="Y182">
+        <v>474</v>
       </c>
     </row>
     <row r="183" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -21694,6 +21891,9 @@
       <c r="X185" t="s">
         <v>1365</v>
       </c>
+      <c r="Y185">
+        <v>167</v>
+      </c>
     </row>
     <row r="186" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
@@ -22455,6 +22655,9 @@
       <c r="X195" t="s">
         <v>1381</v>
       </c>
+      <c r="Y195">
+        <v>191</v>
+      </c>
     </row>
     <row r="196" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
@@ -22529,6 +22732,9 @@
       <c r="X196" t="s">
         <v>1383</v>
       </c>
+      <c r="Y196">
+        <v>185</v>
+      </c>
     </row>
     <row r="197" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
@@ -22604,7 +22810,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="198" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>182</v>
       </c>
@@ -22677,8 +22883,11 @@
       <c r="X198" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="199" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y198">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>183</v>
       </c>
@@ -22750,6 +22959,9 @@
       </c>
       <c r="X199" t="s">
         <v>1387</v>
+      </c>
+      <c r="Y199">
+        <v>479</v>
       </c>
     </row>
     <row r="200" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -23053,6 +23265,9 @@
       <c r="X203" t="s">
         <v>1393</v>
       </c>
+      <c r="Y203">
+        <v>767</v>
+      </c>
     </row>
     <row r="204" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
@@ -23355,8 +23570,11 @@
       <c r="X207" t="s">
         <v>1399</v>
       </c>
-    </row>
-    <row r="208" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y207">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>154</v>
       </c>
@@ -23429,8 +23647,11 @@
       <c r="X208" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y208">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="209" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>413</v>
       </c>
@@ -23578,7 +23799,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -23799,6 +24020,9 @@
       <c r="X213" t="s">
         <v>1409</v>
       </c>
+      <c r="Y213">
+        <v>168</v>
+      </c>
     </row>
     <row r="214" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
@@ -23873,6 +24097,9 @@
       <c r="X214" t="s">
         <v>1409</v>
       </c>
+      <c r="Y214">
+        <v>168</v>
+      </c>
     </row>
     <row r="215" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
@@ -24025,7 +24252,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>213</v>
       </c>
@@ -24172,8 +24399,11 @@
       <c r="X218" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y218">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="219" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -24546,7 +24776,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>212</v>
       </c>
@@ -24620,7 +24850,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>221</v>
       </c>
@@ -24694,7 +24924,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>220</v>
       </c>
@@ -24841,6 +25071,9 @@
       <c r="X227" t="s">
         <v>1433</v>
       </c>
+      <c r="Y227">
+        <v>183</v>
+      </c>
     </row>
     <row r="228" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
@@ -24915,6 +25148,9 @@
       <c r="X228" t="s">
         <v>1433</v>
       </c>
+      <c r="Y228">
+        <v>183</v>
+      </c>
     </row>
     <row r="229" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
@@ -24993,7 +25229,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>346</v>
       </c>
@@ -25070,7 +25306,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>245</v>
       </c>
@@ -25147,7 +25383,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>244</v>
       </c>
@@ -25224,7 +25460,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>251</v>
       </c>
@@ -25301,7 +25537,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>260</v>
       </c>
@@ -25822,7 +26058,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>217</v>
       </c>
@@ -25969,6 +26205,9 @@
       <c r="X242" t="s">
         <v>1453</v>
       </c>
+      <c r="Y242">
+        <v>635</v>
+      </c>
     </row>
     <row r="243" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
@@ -26043,6 +26282,9 @@
       <c r="X243" t="s">
         <v>1455</v>
       </c>
+      <c r="Y243">
+        <v>208</v>
+      </c>
     </row>
     <row r="244" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
@@ -26500,7 +26742,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="250" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>144</v>
       </c>
@@ -26573,8 +26815,11 @@
       <c r="X250" t="s">
         <v>1465</v>
       </c>
-    </row>
-    <row r="251" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y250">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>199</v>
       </c>
@@ -26646,6 +26891,9 @@
       </c>
       <c r="X251" t="s">
         <v>1467</v>
+      </c>
+      <c r="Y251">
+        <v>467</v>
       </c>
     </row>
     <row r="252" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -26722,7 +26970,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>214</v>
       </c>
@@ -26872,8 +27120,11 @@
       <c r="X254" t="s">
         <v>1474</v>
       </c>
-    </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y254">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="255" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>215</v>
       </c>
@@ -27174,6 +27425,9 @@
       <c r="X258" t="s">
         <v>1482</v>
       </c>
+      <c r="Y258">
+        <v>209</v>
+      </c>
     </row>
     <row r="259" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -27702,7 +27956,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="266" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>142</v>
       </c>
@@ -27774,6 +28028,9 @@
       </c>
       <c r="X266" t="s">
         <v>1498</v>
+      </c>
+      <c r="Y266">
+        <v>835</v>
       </c>
     </row>
     <row r="267" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -27850,7 +28107,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>235</v>
       </c>
@@ -28377,7 +28634,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>229</v>
       </c>
@@ -28454,7 +28711,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>276</v>
       </c>
@@ -28752,6 +29009,9 @@
       <c r="X279" t="s">
         <v>1524</v>
       </c>
+      <c r="Y279">
+        <v>206</v>
+      </c>
     </row>
     <row r="280" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
@@ -29051,8 +29311,11 @@
       <c r="X283" t="s">
         <v>1532</v>
       </c>
-    </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y283">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="284" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>216</v>
       </c>
@@ -29202,6 +29465,9 @@
       <c r="X285" t="s">
         <v>1536</v>
       </c>
+      <c r="Y285">
+        <v>197</v>
+      </c>
     </row>
     <row r="286" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
@@ -29277,7 +29543,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="287" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>150</v>
       </c>
@@ -29350,8 +29616,11 @@
       <c r="X287" t="s">
         <v>1540</v>
       </c>
-    </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y287">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="288" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>211</v>
       </c>
@@ -29652,6 +29921,9 @@
       <c r="X291" t="s">
         <v>1546</v>
       </c>
+      <c r="Y291">
+        <v>186</v>
+      </c>
     </row>
     <row r="292" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
@@ -30263,7 +30535,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="300" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>28</v>
       </c>
@@ -30335,6 +30607,9 @@
       </c>
       <c r="X300" t="s">
         <v>1562</v>
+      </c>
+      <c r="Y300">
+        <v>740</v>
       </c>
     </row>
     <row r="301" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -30793,7 +31068,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>417</v>
       </c>
@@ -30867,7 +31142,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>227</v>
       </c>
@@ -30941,7 +31216,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>226</v>
       </c>
@@ -31391,7 +31666,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>262</v>
       </c>
@@ -31840,6 +32115,9 @@
       <c r="X320" t="s">
         <v>1596</v>
       </c>
+      <c r="Y320">
+        <v>192</v>
+      </c>
     </row>
     <row r="321" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
@@ -31914,6 +32192,9 @@
       <c r="X321" t="s">
         <v>1596</v>
       </c>
+      <c r="Y321">
+        <v>192</v>
+      </c>
     </row>
     <row r="322" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
@@ -31988,6 +32269,9 @@
       <c r="X322" t="s">
         <v>1598</v>
       </c>
+      <c r="Y322">
+        <v>201</v>
+      </c>
     </row>
     <row r="323" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
@@ -32216,8 +32500,11 @@
       <c r="X325" t="s">
         <v>1604</v>
       </c>
-    </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y325">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="326" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>356</v>
       </c>
@@ -32367,6 +32654,9 @@
       <c r="X327" t="s">
         <v>1608</v>
       </c>
+      <c r="Y327">
+        <v>169</v>
+      </c>
     </row>
     <row r="328" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
@@ -32740,6 +33030,9 @@
       <c r="X332" t="s">
         <v>1616</v>
       </c>
+      <c r="Y332">
+        <v>207</v>
+      </c>
     </row>
     <row r="333" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
@@ -32968,6 +33261,9 @@
       <c r="X335" t="s">
         <v>1622</v>
       </c>
+      <c r="Y335">
+        <v>194</v>
+      </c>
     </row>
     <row r="336" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -33042,6 +33338,9 @@
       <c r="X336" t="s">
         <v>1622</v>
       </c>
+      <c r="Y336">
+        <v>194</v>
+      </c>
     </row>
     <row r="337" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
@@ -33116,6 +33415,9 @@
       <c r="X337" t="s">
         <v>1624</v>
       </c>
+      <c r="Y337">
+        <v>195</v>
+      </c>
     </row>
     <row r="338" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
@@ -33190,6 +33492,9 @@
       <c r="X338" t="s">
         <v>1624</v>
       </c>
+      <c r="Y338">
+        <v>195</v>
+      </c>
     </row>
     <row r="339" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
@@ -33419,7 +33724,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="342" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>168</v>
       </c>
@@ -33491,6 +33796,9 @@
       </c>
       <c r="X342" t="s">
         <v>1632</v>
+      </c>
+      <c r="Y342">
+        <v>477</v>
       </c>
     </row>
     <row r="343" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -33567,7 +33875,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="344" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>147</v>
       </c>
@@ -33640,8 +33948,11 @@
       <c r="X344" t="s">
         <v>1636</v>
       </c>
-    </row>
-    <row r="345" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y344">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>146</v>
       </c>
@@ -33714,8 +34025,11 @@
       <c r="X345" t="s">
         <v>1636</v>
       </c>
-    </row>
-    <row r="346" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y345">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>145</v>
       </c>
@@ -33787,6 +34101,9 @@
       </c>
       <c r="X346" t="s">
         <v>1636</v>
+      </c>
+      <c r="Y346">
+        <v>478</v>
       </c>
     </row>
     <row r="347" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -33862,8 +34179,11 @@
       <c r="X347" t="s">
         <v>1638</v>
       </c>
-    </row>
-    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y347">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="348" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>265</v>
       </c>
@@ -33937,7 +34257,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>266</v>
       </c>
@@ -34011,7 +34331,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>263</v>
       </c>
@@ -34386,8 +34706,11 @@
       <c r="X354" t="s">
         <v>1648</v>
       </c>
-    </row>
-    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y354">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="355" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>261</v>
       </c>
@@ -34464,7 +34787,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>257</v>
       </c>
@@ -34541,7 +34864,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>264</v>
       </c>
@@ -34618,7 +34941,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="358" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>31</v>
       </c>
@@ -34691,8 +35014,11 @@
       <c r="X358" t="s">
         <v>1652</v>
       </c>
-    </row>
-    <row r="359" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y358">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>29</v>
       </c>
@@ -34765,8 +35091,11 @@
       <c r="X359" t="s">
         <v>1652</v>
       </c>
-    </row>
-    <row r="360" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y359">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>30</v>
       </c>
@@ -34838,6 +35167,9 @@
       </c>
       <c r="X360" t="s">
         <v>1652</v>
+      </c>
+      <c r="Y360">
+        <v>443</v>
       </c>
     </row>
     <row r="361" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -34914,7 +35246,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="362" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>33</v>
       </c>
@@ -34987,8 +35319,11 @@
       <c r="X362" t="s">
         <v>1656</v>
       </c>
-    </row>
-    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y362">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="363" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>207</v>
       </c>
@@ -35209,6 +35544,9 @@
       <c r="X365" t="s">
         <v>1662</v>
       </c>
+      <c r="Y365">
+        <v>639</v>
+      </c>
     </row>
     <row r="366" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
@@ -35431,8 +35769,11 @@
       <c r="X368" t="s">
         <v>1668</v>
       </c>
-    </row>
-    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y368">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="369" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>228</v>
       </c>
@@ -36174,6 +36515,9 @@
       <c r="X378" t="s">
         <v>1686</v>
       </c>
+      <c r="Y378">
+        <v>165</v>
+      </c>
     </row>
     <row r="379" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
@@ -36248,6 +36592,9 @@
       <c r="X379" t="s">
         <v>1686</v>
       </c>
+      <c r="Y379">
+        <v>165</v>
+      </c>
     </row>
     <row r="380" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
@@ -36399,6 +36746,9 @@
       <c r="X381" t="s">
         <v>1690</v>
       </c>
+      <c r="Y381">
+        <v>200</v>
+      </c>
     </row>
     <row r="382" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -36477,7 +36827,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>208</v>
       </c>
@@ -36551,7 +36901,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="384" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>174</v>
       </c>
@@ -36624,8 +36974,11 @@
       <c r="X384" t="s">
         <v>1696</v>
       </c>
-    </row>
-    <row r="385" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y384">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>176</v>
       </c>
@@ -36698,8 +37051,11 @@
       <c r="X385" t="s">
         <v>1696</v>
       </c>
-    </row>
-    <row r="386" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y385">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>178</v>
       </c>
@@ -36771,6 +37127,9 @@
       </c>
       <c r="X386" t="s">
         <v>1696</v>
+      </c>
+      <c r="Y386">
+        <v>480</v>
       </c>
     </row>
     <row r="387" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -36846,6 +37205,9 @@
       <c r="X387" t="s">
         <v>1698</v>
       </c>
+      <c r="Y387">
+        <v>177</v>
+      </c>
     </row>
     <row r="388" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
@@ -36920,6 +37282,9 @@
       <c r="X388" t="s">
         <v>1698</v>
       </c>
+      <c r="Y388">
+        <v>177</v>
+      </c>
     </row>
     <row r="389" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
@@ -37518,6 +37883,9 @@
       <c r="X396" t="s">
         <v>1712</v>
       </c>
+      <c r="Y396">
+        <v>211</v>
+      </c>
     </row>
     <row r="397" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
@@ -37823,6 +38191,9 @@
       <c r="X400" t="s">
         <v>1720</v>
       </c>
+      <c r="Y400">
+        <v>584</v>
+      </c>
     </row>
     <row r="401" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
@@ -37975,7 +38346,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="403" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>172</v>
       </c>
@@ -38048,8 +38419,11 @@
       <c r="X403" t="s">
         <v>1726</v>
       </c>
-    </row>
-    <row r="404" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y403">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="404" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>159</v>
       </c>
@@ -38121,6 +38495,9 @@
       </c>
       <c r="X404" t="s">
         <v>1726</v>
+      </c>
+      <c r="Y404">
+        <v>465</v>
       </c>
     </row>
     <row r="405" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
@@ -38270,6 +38647,9 @@
       <c r="X406" t="s">
         <v>1730</v>
       </c>
+      <c r="Y406">
+        <v>196</v>
+      </c>
     </row>
     <row r="407" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
@@ -39709,6 +40089,9 @@
       <c r="X425" t="s">
         <v>1758</v>
       </c>
+      <c r="Y425">
+        <v>176</v>
+      </c>
     </row>
     <row r="426" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
@@ -40005,6 +40388,9 @@
       <c r="X429" t="s">
         <v>1764</v>
       </c>
+      <c r="Y429">
+        <v>189</v>
+      </c>
     </row>
     <row r="430" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
@@ -40228,7 +40614,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="433" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>347</v>
       </c>
@@ -40605,7 +40991,7 @@
   <autoFilter ref="A1:Y437" xr:uid="{A5B3DFC9-D175-4697-87AC-4A141BB6D52C}">
     <filterColumn colId="20">
       <filters>
-        <filter val="Financeiros"/>
+        <filter val="Utilidade Pública"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A74:Y424">

</xml_diff>

<commit_message>
[Em Andamento] Frontend configurações iniciais
</commit_message>
<xml_diff>
--- a/src/infoinvestbr/src/analise/rendavariavel.xlsx
+++ b/src/infoinvestbr/src/analise/rendavariavel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\Projeto TCC\src\infoinvestbr\src\analise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA02586E-E46C-424E-99DF-0EAD882BBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA69F2F-7F91-4349-9217-6006298F45BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{FE4D7603-F5DE-4554-98D0-6C8EE02FCDF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FE4D7603-F5DE-4554-98D0-6C8EE02FCDF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ações" sheetId="1" r:id="rId1"/>
@@ -7758,12 +7758,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B3DFC9-D175-4697-87AC-4A141BB6D52C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Y437"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="A1:Y1"/>
-    </sheetView>
+    <sheetView topLeftCell="N1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7871,7 +7868,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>393</v>
       </c>
@@ -7948,7 +7945,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>241</v>
       </c>
@@ -8025,7 +8022,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -8102,7 +8099,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>287</v>
       </c>
@@ -8333,7 +8330,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8410,7 +8407,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -8487,7 +8484,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="10" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -8561,7 +8558,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="11" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>457</v>
       </c>
@@ -8635,7 +8632,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="12" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>456</v>
       </c>
@@ -8709,7 +8706,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="13" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>405</v>
       </c>
@@ -8786,7 +8783,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>219</v>
       </c>
@@ -9094,7 +9091,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -9245,7 +9242,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -9319,7 +9316,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -9393,7 +9390,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>358</v>
       </c>
@@ -9470,7 +9467,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -9544,7 +9541,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -9618,7 +9615,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -9692,7 +9689,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>406</v>
       </c>
@@ -9769,7 +9766,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>327</v>
       </c>
@@ -9923,7 +9920,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="29" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -9997,7 +9994,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="30" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>126</v>
       </c>
@@ -10074,7 +10071,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -10151,7 +10148,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>471</v>
       </c>
@@ -10228,7 +10225,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>416</v>
       </c>
@@ -10305,7 +10302,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -10379,7 +10376,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>204</v>
       </c>
@@ -10456,7 +10453,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>205</v>
       </c>
@@ -10533,7 +10530,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -10607,7 +10604,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -10684,7 +10681,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>238</v>
       </c>
@@ -10761,7 +10758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>248</v>
       </c>
@@ -10838,7 +10835,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>255</v>
       </c>
@@ -10915,7 +10912,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>354</v>
       </c>
@@ -10992,7 +10989,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>295</v>
       </c>
@@ -11069,7 +11066,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>292</v>
       </c>
@@ -11146,7 +11143,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -11220,7 +11217,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>249</v>
       </c>
@@ -11297,7 +11294,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>256</v>
       </c>
@@ -11374,7 +11371,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>239</v>
       </c>
@@ -11451,7 +11448,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>318</v>
       </c>
@@ -11528,7 +11525,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>81</v>
       </c>
@@ -11602,7 +11599,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="51" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -11679,7 +11676,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>242</v>
       </c>
@@ -11756,7 +11753,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>243</v>
       </c>
@@ -11833,7 +11830,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>269</v>
       </c>
@@ -11910,7 +11907,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>252</v>
       </c>
@@ -11987,7 +11984,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>493</v>
       </c>
@@ -12061,7 +12058,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="57" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>370</v>
       </c>
@@ -12138,7 +12135,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -12212,7 +12209,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>415</v>
       </c>
@@ -12286,7 +12283,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -12360,7 +12357,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>270</v>
       </c>
@@ -12437,7 +12434,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>274</v>
       </c>
@@ -12514,7 +12511,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -12591,7 +12588,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>268</v>
       </c>
@@ -12668,7 +12665,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>323</v>
       </c>
@@ -12745,7 +12742,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>324</v>
       </c>
@@ -12822,7 +12819,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="67" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>259</v>
       </c>
@@ -12899,7 +12896,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -12973,7 +12970,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>348</v>
       </c>
@@ -13050,7 +13047,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>352</v>
       </c>
@@ -13127,7 +13124,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>350</v>
       </c>
@@ -13204,7 +13201,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>353</v>
       </c>
@@ -13281,7 +13278,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>351</v>
       </c>
@@ -13358,7 +13355,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>467</v>
       </c>
@@ -13435,7 +13432,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="75" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -13512,7 +13509,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>254</v>
       </c>
@@ -13589,7 +13586,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>386</v>
       </c>
@@ -13666,7 +13663,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>384</v>
       </c>
@@ -13743,7 +13740,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>385</v>
       </c>
@@ -13820,7 +13817,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -13897,7 +13894,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>250</v>
       </c>
@@ -13974,7 +13971,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>267</v>
       </c>
@@ -14051,7 +14048,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>246</v>
       </c>
@@ -14128,7 +14125,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="84" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>275</v>
       </c>
@@ -14205,7 +14202,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>273</v>
       </c>
@@ -14282,7 +14279,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="86" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>106</v>
       </c>
@@ -14356,7 +14353,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="87" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>447</v>
       </c>
@@ -14430,7 +14427,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="88" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>40</v>
       </c>
@@ -14504,7 +14501,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="89" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>363</v>
       </c>
@@ -14581,7 +14578,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>326</v>
       </c>
@@ -14735,7 +14732,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="92" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>473</v>
       </c>
@@ -14812,7 +14809,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -15117,7 +15114,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="97" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>436</v>
       </c>
@@ -15191,7 +15188,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="98" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>438</v>
       </c>
@@ -15650,7 +15647,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="104" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>64</v>
       </c>
@@ -15724,7 +15721,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="105" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>63</v>
       </c>
@@ -15798,7 +15795,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="106" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>414</v>
       </c>
@@ -15875,7 +15872,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>412</v>
       </c>
@@ -16257,7 +16254,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="112" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>328</v>
       </c>
@@ -16488,7 +16485,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -16947,7 +16944,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="121" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>96</v>
       </c>
@@ -17021,7 +17018,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="122" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>82</v>
       </c>
@@ -17095,7 +17092,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="123" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>271</v>
       </c>
@@ -17172,7 +17169,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="124" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>272</v>
       </c>
@@ -17249,7 +17246,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="125" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>388</v>
       </c>
@@ -17326,7 +17323,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="126" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>387</v>
       </c>
@@ -17403,7 +17400,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="127" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>355</v>
       </c>
@@ -17480,7 +17477,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="128" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>357</v>
       </c>
@@ -17557,7 +17554,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="129" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>342</v>
       </c>
@@ -17634,7 +17631,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="130" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>138</v>
       </c>
@@ -17785,7 +17782,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="132" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>431</v>
       </c>
@@ -18093,7 +18090,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>407</v>
       </c>
@@ -18170,7 +18167,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>435</v>
       </c>
@@ -18244,7 +18241,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="138" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>442</v>
       </c>
@@ -18318,7 +18315,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="139" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>444</v>
       </c>
@@ -18392,7 +18389,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="140" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>439</v>
       </c>
@@ -18466,7 +18463,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="141" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>440</v>
       </c>
@@ -18540,7 +18537,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="142" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>116</v>
       </c>
@@ -18614,7 +18611,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="143" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>492</v>
       </c>
@@ -18688,7 +18685,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="144" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>349</v>
       </c>
@@ -18765,7 +18762,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="145" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>110</v>
       </c>
@@ -18839,7 +18836,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="146" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>394</v>
       </c>
@@ -18916,7 +18913,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="147" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>464</v>
       </c>
@@ -18993,7 +18990,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="148" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>383</v>
       </c>
@@ -19070,7 +19067,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="149" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>380</v>
       </c>
@@ -19147,7 +19144,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="150" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>117</v>
       </c>
@@ -19221,7 +19218,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="151" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>240</v>
       </c>
@@ -19295,7 +19292,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="152" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>84</v>
       </c>
@@ -19369,7 +19366,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="153" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>453</v>
       </c>
@@ -19443,7 +19440,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="154" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>134</v>
       </c>
@@ -19517,7 +19514,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="155" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>403</v>
       </c>
@@ -19594,7 +19591,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="156" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>285</v>
       </c>
@@ -19671,7 +19668,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="157" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>298</v>
       </c>
@@ -19748,7 +19745,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="158" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>296</v>
       </c>
@@ -19825,7 +19822,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="159" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>478</v>
       </c>
@@ -20364,7 +20361,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="166" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>321</v>
       </c>
@@ -20518,7 +20515,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>307</v>
       </c>
@@ -20595,7 +20592,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>337</v>
       </c>
@@ -21057,7 +21054,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="175" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>367</v>
       </c>
@@ -21288,7 +21285,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="178" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>62</v>
       </c>
@@ -21670,7 +21667,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="183" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>55</v>
       </c>
@@ -21744,7 +21741,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="184" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>491</v>
       </c>
@@ -21818,7 +21815,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="185" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>121</v>
       </c>
@@ -21895,7 +21892,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="186" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>278</v>
       </c>
@@ -21972,7 +21969,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="187" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>279</v>
       </c>
@@ -22049,7 +22046,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="188" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>109</v>
       </c>
@@ -22123,7 +22120,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="189" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>114</v>
       </c>
@@ -22197,7 +22194,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="190" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>427</v>
       </c>
@@ -22274,7 +22271,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="191" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>426</v>
       </c>
@@ -22351,7 +22348,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="192" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>377</v>
       </c>
@@ -22428,7 +22425,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="193" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>463</v>
       </c>
@@ -22505,7 +22502,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="194" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>399</v>
       </c>
@@ -22582,7 +22579,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="195" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>316</v>
       </c>
@@ -22659,7 +22656,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>289</v>
       </c>
@@ -22736,7 +22733,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="197" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>21</v>
       </c>
@@ -22964,7 +22961,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="200" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>95</v>
       </c>
@@ -23038,7 +23035,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="201" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>423</v>
       </c>
@@ -23115,7 +23112,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="202" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>424</v>
       </c>
@@ -23192,7 +23189,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="203" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>409</v>
       </c>
@@ -23269,7 +23266,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="204" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>80</v>
       </c>
@@ -23343,7 +23340,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="205" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>421</v>
       </c>
@@ -23420,7 +23417,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="206" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>422</v>
       </c>
@@ -23497,7 +23494,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="207" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>472</v>
       </c>
@@ -23651,7 +23648,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="209" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>413</v>
       </c>
@@ -23725,7 +23722,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="210" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>452</v>
       </c>
@@ -23799,7 +23796,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="211" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -23873,7 +23870,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="212" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>73</v>
       </c>
@@ -23947,7 +23944,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="213" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>125</v>
       </c>
@@ -24024,7 +24021,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="214" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>120</v>
       </c>
@@ -24101,7 +24098,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="215" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>392</v>
       </c>
@@ -24178,7 +24175,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="216" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>107</v>
       </c>
@@ -24252,7 +24249,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="217" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>213</v>
       </c>
@@ -24326,7 +24323,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="218" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>470</v>
       </c>
@@ -24403,7 +24400,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="219" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -24477,7 +24474,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="220" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>484</v>
       </c>
@@ -24551,7 +24548,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="221" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>233</v>
       </c>
@@ -24625,7 +24622,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="222" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>83</v>
       </c>
@@ -24699,7 +24696,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="223" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>368</v>
       </c>
@@ -24776,7 +24773,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="224" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>212</v>
       </c>
@@ -24850,7 +24847,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="225" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>221</v>
       </c>
@@ -24924,7 +24921,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="226" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>220</v>
       </c>
@@ -24998,7 +24995,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="227" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>291</v>
       </c>
@@ -25075,7 +25072,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="228" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>290</v>
       </c>
@@ -25152,7 +25149,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="229" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>92</v>
       </c>
@@ -25229,7 +25226,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="230" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>346</v>
       </c>
@@ -25306,7 +25303,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="231" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>245</v>
       </c>
@@ -25383,7 +25380,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="232" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>244</v>
       </c>
@@ -25460,7 +25457,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="233" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>251</v>
       </c>
@@ -25537,7 +25534,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="234" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>260</v>
       </c>
@@ -25614,7 +25611,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="235" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>39</v>
       </c>
@@ -25688,7 +25685,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="236" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>38</v>
       </c>
@@ -25762,7 +25759,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="237" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>100</v>
       </c>
@@ -25836,7 +25833,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="238" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>105</v>
       </c>
@@ -25910,7 +25907,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="239" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>41</v>
       </c>
@@ -25984,7 +25981,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="240" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>45</v>
       </c>
@@ -26058,7 +26055,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="241" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>217</v>
       </c>
@@ -26132,7 +26129,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="242" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>475</v>
       </c>
@@ -26209,7 +26206,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="243" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>299</v>
       </c>
@@ -26286,7 +26283,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="244" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>281</v>
       </c>
@@ -26363,7 +26360,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="245" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>283</v>
       </c>
@@ -26440,7 +26437,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="246" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>282</v>
       </c>
@@ -26517,7 +26514,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="247" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>395</v>
       </c>
@@ -26594,7 +26591,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="248" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>112</v>
       </c>
@@ -26668,7 +26665,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="249" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>50</v>
       </c>
@@ -26896,7 +26893,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="252" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>56</v>
       </c>
@@ -26970,7 +26967,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="253" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>214</v>
       </c>
@@ -27047,7 +27044,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="254" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>477</v>
       </c>
@@ -27124,7 +27121,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>215</v>
       </c>
@@ -27201,7 +27198,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="256" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>69</v>
       </c>
@@ -27275,7 +27272,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="257" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>332</v>
       </c>
@@ -27352,7 +27349,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="258" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>481</v>
       </c>
@@ -27429,7 +27426,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="259" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>371</v>
       </c>
@@ -27506,7 +27503,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="260" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>375</v>
       </c>
@@ -27583,7 +27580,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="261" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>400</v>
       </c>
@@ -27660,7 +27657,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="262" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>366</v>
       </c>
@@ -27734,7 +27731,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="263" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>46</v>
       </c>
@@ -27808,7 +27805,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="264" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>104</v>
       </c>
@@ -27882,7 +27879,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="265" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>232</v>
       </c>
@@ -28033,7 +28030,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="267" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>108</v>
       </c>
@@ -28107,7 +28104,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="268" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>235</v>
       </c>
@@ -28184,7 +28181,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="269" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>420</v>
       </c>
@@ -28261,7 +28258,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="270" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>54</v>
       </c>
@@ -28335,7 +28332,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="271" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>136</v>
       </c>
@@ -28409,7 +28406,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="272" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>90</v>
       </c>
@@ -28486,7 +28483,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="273" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>443</v>
       </c>
@@ -28560,7 +28557,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="274" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>43</v>
       </c>
@@ -28634,7 +28631,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="275" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>229</v>
       </c>
@@ -28711,7 +28708,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="276" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>276</v>
       </c>
@@ -28788,7 +28785,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="277" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>135</v>
       </c>
@@ -28862,7 +28859,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="278" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>37</v>
       </c>
@@ -28936,7 +28933,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="279" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>476</v>
       </c>
@@ -29013,7 +29010,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="280" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>94</v>
       </c>
@@ -29087,7 +29084,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="281" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>277</v>
       </c>
@@ -29164,7 +29161,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="282" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>115</v>
       </c>
@@ -29238,7 +29235,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="283" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>297</v>
       </c>
@@ -29315,7 +29312,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="284" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>216</v>
       </c>
@@ -29392,7 +29389,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="285" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>309</v>
       </c>
@@ -29469,7 +29466,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="286" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>49</v>
       </c>
@@ -29620,7 +29617,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="288" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>211</v>
       </c>
@@ -29694,7 +29691,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="289" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>372</v>
       </c>
@@ -29771,7 +29768,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="290" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>364</v>
       </c>
@@ -29848,7 +29845,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="291" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>288</v>
       </c>
@@ -29925,7 +29922,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="292" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>360</v>
       </c>
@@ -29999,7 +29996,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="293" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>381</v>
       </c>
@@ -30076,7 +30073,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="294" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>397</v>
       </c>
@@ -30153,7 +30150,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="295" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>319</v>
       </c>
@@ -30230,7 +30227,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="296" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>462</v>
       </c>
@@ -30307,7 +30304,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="297" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>461</v>
       </c>
@@ -30384,7 +30381,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="298" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>391</v>
       </c>
@@ -30461,7 +30458,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="299" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>331</v>
       </c>
@@ -30612,7 +30609,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="301" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>334</v>
       </c>
@@ -30689,7 +30686,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="302" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>398</v>
       </c>
@@ -30766,7 +30763,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="303" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>433</v>
       </c>
@@ -30843,7 +30840,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="304" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>432</v>
       </c>
@@ -30920,7 +30917,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="305" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>77</v>
       </c>
@@ -30994,7 +30991,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="306" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>103</v>
       </c>
@@ -31068,7 +31065,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="307" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>417</v>
       </c>
@@ -31142,7 +31139,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="308" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>227</v>
       </c>
@@ -31216,7 +31213,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="309" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>226</v>
       </c>
@@ -31290,7 +31287,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="310" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>336</v>
       </c>
@@ -31367,7 +31364,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="311" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>335</v>
       </c>
@@ -31444,7 +31441,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="312" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>74</v>
       </c>
@@ -31518,7 +31515,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="313" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>78</v>
       </c>
@@ -31592,7 +31589,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="314" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>79</v>
       </c>
@@ -31666,7 +31663,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="315" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>262</v>
       </c>
@@ -31743,7 +31740,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="316" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>48</v>
       </c>
@@ -31817,7 +31814,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="317" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>111</v>
       </c>
@@ -31891,7 +31888,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="318" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>419</v>
       </c>
@@ -31968,7 +31965,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="319" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>85</v>
       </c>
@@ -32042,7 +32039,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="320" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>312</v>
       </c>
@@ -32119,7 +32116,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="321" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>315</v>
       </c>
@@ -32196,7 +32193,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="322" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>479</v>
       </c>
@@ -32273,7 +32270,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="323" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>91</v>
       </c>
@@ -32350,7 +32347,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="324" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>339</v>
       </c>
@@ -32427,7 +32424,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>408</v>
       </c>
@@ -32504,7 +32501,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="326" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>356</v>
       </c>
@@ -32581,7 +32578,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="327" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>122</v>
       </c>
@@ -32658,7 +32655,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="328" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>451</v>
       </c>
@@ -32732,7 +32729,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="329" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>449</v>
       </c>
@@ -32806,7 +32803,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="330" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>396</v>
       </c>
@@ -32883,7 +32880,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="331" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>88</v>
       </c>
@@ -32957,7 +32954,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="332" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>482</v>
       </c>
@@ -33034,7 +33031,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="333" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>344</v>
       </c>
@@ -33111,7 +33108,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="334" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>284</v>
       </c>
@@ -33188,7 +33185,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="335" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>310</v>
       </c>
@@ -33265,7 +33262,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="336" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>311</v>
       </c>
@@ -33342,7 +33339,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="337" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>306</v>
       </c>
@@ -33419,7 +33416,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="338" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>308</v>
       </c>
@@ -33496,7 +33493,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="339" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>118</v>
       </c>
@@ -33570,7 +33567,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="340" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>401</v>
       </c>
@@ -33647,7 +33644,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="341" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>338</v>
       </c>
@@ -33801,7 +33798,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="343" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>139</v>
       </c>
@@ -34106,7 +34103,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="347" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>301</v>
       </c>
@@ -34183,7 +34180,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="348" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>265</v>
       </c>
@@ -34257,7 +34254,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="349" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>266</v>
       </c>
@@ -34331,7 +34328,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="350" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>263</v>
       </c>
@@ -34405,7 +34402,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="351" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>333</v>
       </c>
@@ -34482,7 +34479,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="352" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>343</v>
       </c>
@@ -34559,7 +34556,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="353" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>101</v>
       </c>
@@ -34633,7 +34630,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="354" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>313</v>
       </c>
@@ -34710,7 +34707,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="355" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>261</v>
       </c>
@@ -34787,7 +34784,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="356" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>257</v>
       </c>
@@ -34864,7 +34861,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="357" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>264</v>
       </c>
@@ -35172,7 +35169,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="361" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>68</v>
       </c>
@@ -35323,7 +35320,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="363" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>207</v>
       </c>
@@ -35397,7 +35394,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="364" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>131</v>
       </c>
@@ -35471,7 +35468,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="365" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>404</v>
       </c>
@@ -35548,7 +35545,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="366" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>445</v>
       </c>
@@ -35622,7 +35619,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="367" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>490</v>
       </c>
@@ -35696,7 +35693,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="368" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>300</v>
       </c>
@@ -35773,7 +35770,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="369" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>228</v>
       </c>
@@ -35847,7 +35844,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="370" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>22</v>
       </c>
@@ -35921,7 +35918,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="371" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>61</v>
       </c>
@@ -35995,7 +35992,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="372" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>60</v>
       </c>
@@ -36069,7 +36066,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="373" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>489</v>
       </c>
@@ -36143,7 +36140,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="374" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>42</v>
       </c>
@@ -36217,7 +36214,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="375" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>304</v>
       </c>
@@ -36294,7 +36291,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="376" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>24</v>
       </c>
@@ -36368,7 +36365,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="377" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>71</v>
       </c>
@@ -36442,7 +36439,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="378" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>124</v>
       </c>
@@ -36519,7 +36516,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="379" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>123</v>
       </c>
@@ -36596,7 +36593,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="380" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>374</v>
       </c>
@@ -36673,7 +36670,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="381" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>480</v>
       </c>
@@ -36750,7 +36747,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="382" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>280</v>
       </c>
@@ -36827,7 +36824,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="383" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>208</v>
       </c>
@@ -37132,7 +37129,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="387" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>294</v>
       </c>
@@ -37209,7 +37206,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="388" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>293</v>
       </c>
@@ -37286,7 +37283,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="389" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>98</v>
       </c>
@@ -37360,7 +37357,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="390" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>448</v>
       </c>
@@ -37434,7 +37431,7 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="391" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>446</v>
       </c>
@@ -37508,7 +37505,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="392" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>459</v>
       </c>
@@ -37585,7 +37582,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="393" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>460</v>
       </c>
@@ -37662,7 +37659,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="394" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>99</v>
       </c>
@@ -37736,7 +37733,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="395" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>455</v>
       </c>
@@ -37810,7 +37807,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="396" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>474</v>
       </c>
@@ -37887,7 +37884,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="397" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>466</v>
       </c>
@@ -37964,7 +37961,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="398" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>425</v>
       </c>
@@ -38041,7 +38038,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="399" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>373</v>
       </c>
@@ -38118,7 +38115,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="400" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>469</v>
       </c>
@@ -38195,7 +38192,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="401" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>365</v>
       </c>
@@ -38272,7 +38269,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="402" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>113</v>
       </c>
@@ -38500,7 +38497,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="405" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>23</v>
       </c>
@@ -38574,7 +38571,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="406" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>314</v>
       </c>
@@ -38651,7 +38648,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="407" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>437</v>
       </c>
@@ -38725,7 +38722,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="408" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>441</v>
       </c>
@@ -38799,7 +38796,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="409" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>485</v>
       </c>
@@ -38873,7 +38870,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="410" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>340</v>
       </c>
@@ -38950,7 +38947,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="411" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>378</v>
       </c>
@@ -39027,7 +39024,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="412" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>382</v>
       </c>
@@ -39104,7 +39101,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="413" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>379</v>
       </c>
@@ -39181,7 +39178,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="414" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>429</v>
       </c>
@@ -39258,7 +39255,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="415" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>428</v>
       </c>
@@ -39335,7 +39332,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="416" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>430</v>
       </c>
@@ -39412,7 +39409,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="417" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>325</v>
       </c>
@@ -39489,7 +39486,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="418" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>137</v>
       </c>
@@ -39563,7 +39560,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="419" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>341</v>
       </c>
@@ -39640,7 +39637,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="420" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>57</v>
       </c>
@@ -39714,7 +39711,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="421" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>389</v>
       </c>
@@ -39791,7 +39788,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="422" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>454</v>
       </c>
@@ -39865,7 +39862,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="423" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>97</v>
       </c>
@@ -39939,7 +39936,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="424" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>465</v>
       </c>
@@ -40016,7 +40013,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="425" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>410</v>
       </c>
@@ -40093,7 +40090,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="426" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>58</v>
       </c>
@@ -40167,7 +40164,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="427" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>450</v>
       </c>
@@ -40241,7 +40238,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="428" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>86</v>
       </c>
@@ -40315,7 +40312,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="429" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>302</v>
       </c>
@@ -40392,7 +40389,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="430" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>369</v>
       </c>
@@ -40466,7 +40463,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="431" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>487</v>
       </c>
@@ -40540,7 +40537,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="432" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>486</v>
       </c>
@@ -40614,7 +40611,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="433" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>347</v>
       </c>
@@ -40691,7 +40688,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="434" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>66</v>
       </c>
@@ -40765,7 +40762,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="435" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>67</v>
       </c>
@@ -40839,7 +40836,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="436" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>129</v>
       </c>
@@ -40913,7 +40910,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="437" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>231</v>
       </c>
@@ -40988,16 +40985,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y437" xr:uid="{A5B3DFC9-D175-4697-87AC-4A141BB6D52C}">
-    <filterColumn colId="20">
-      <filters>
-        <filter val="Utilidade Pública"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A74:Y424">
-      <sortCondition ref="A1:A437"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="A38">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
@@ -41013,7 +41000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83DC6A1-0485-4D47-A981-9EDF9FDFD333}">
   <dimension ref="A1:V307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>